<commit_message>
completing reports for laterality
</commit_message>
<xml_diff>
--- a/notebooks/data/data_info.xlsx
+++ b/notebooks/data/data_info.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeta\Documents\acou_sommeil_HD_ENS\Tinnitus-n-Sleep\drafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeta\Documents\acou_sommeil_HD_ENS\Tinnitus-n-Sleep\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B35C97E8-088E-4A82-B419-AC81372AD868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B424D4B-3118-4DA0-8DE6-B1790EEC47D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -967,7 +978,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1801,11 +1812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K52" workbookViewId="0">
-      <selection activeCell="N60" sqref="N60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1930,6 +1941,16 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I57" si="0">F2</f>
+        <v>0</v>
+      </c>
       <c r="N2" t="s">
         <v>36</v>
       </c>
@@ -2010,6 +2031,16 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N3" t="s">
         <v>36</v>
       </c>
@@ -2090,6 +2121,16 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N4" t="s">
         <v>36</v>
       </c>
@@ -2170,6 +2211,16 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N5" t="s">
         <v>36</v>
       </c>
@@ -2250,6 +2301,16 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N6" t="s">
         <v>36</v>
       </c>
@@ -2330,6 +2391,16 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N7" t="s">
         <v>36</v>
       </c>
@@ -2410,6 +2481,16 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N8" t="s">
         <v>36</v>
       </c>
@@ -2490,6 +2571,16 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N9" t="s">
         <v>36</v>
       </c>
@@ -2570,6 +2661,16 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N10" t="s">
         <v>36</v>
       </c>
@@ -2650,6 +2751,16 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O11">
         <v>1</v>
       </c>
@@ -2727,6 +2838,16 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N12" t="s">
         <v>98</v>
       </c>
@@ -2807,6 +2928,16 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N13" t="s">
         <v>36</v>
       </c>
@@ -2887,6 +3018,16 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N14" t="s">
         <v>110</v>
       </c>
@@ -2967,6 +3108,16 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N15" t="s">
         <v>36</v>
       </c>
@@ -3047,6 +3198,16 @@
       <c r="F16">
         <v>0</v>
       </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N16" t="s">
         <v>115</v>
       </c>
@@ -3127,6 +3288,16 @@
       <c r="F17">
         <v>0</v>
       </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N17" t="s">
         <v>36</v>
       </c>
@@ -3207,6 +3378,16 @@
       <c r="F18">
         <v>0</v>
       </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N18" t="s">
         <v>36</v>
       </c>
@@ -3287,6 +3468,16 @@
       <c r="F19">
         <v>0</v>
       </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N19" t="s">
         <v>36</v>
       </c>
@@ -3367,6 +3558,16 @@
       <c r="F20">
         <v>0</v>
       </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N20" t="s">
         <v>36</v>
       </c>
@@ -3447,6 +3648,16 @@
       <c r="F21">
         <v>0</v>
       </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N21" t="s">
         <v>36</v>
       </c>
@@ -3527,6 +3738,16 @@
       <c r="F22">
         <v>0</v>
       </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N22" t="s">
         <v>36</v>
       </c>
@@ -3607,6 +3828,16 @@
       <c r="F23">
         <v>0</v>
       </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N23" t="s">
         <v>36</v>
       </c>
@@ -3687,6 +3918,16 @@
       <c r="F24">
         <v>1</v>
       </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N24" t="s">
         <v>152</v>
       </c>
@@ -3767,6 +4008,16 @@
       <c r="F25">
         <v>0</v>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N25" t="s">
         <v>36</v>
       </c>
@@ -3847,6 +4098,16 @@
       <c r="F26">
         <v>0</v>
       </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N26" t="s">
         <v>36</v>
       </c>
@@ -3927,6 +4188,16 @@
       <c r="F27">
         <v>0</v>
       </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N27" t="s">
         <v>36</v>
       </c>
@@ -4007,6 +4278,16 @@
       <c r="F28">
         <v>0</v>
       </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N28" t="s">
         <v>36</v>
       </c>
@@ -4087,6 +4368,16 @@
       <c r="F29">
         <v>0</v>
       </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N29" t="s">
         <v>36</v>
       </c>
@@ -4167,6 +4458,16 @@
       <c r="F30">
         <v>1</v>
       </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O30">
         <v>1</v>
       </c>
@@ -4244,6 +4545,16 @@
       <c r="F31">
         <v>1</v>
       </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O31">
         <v>1</v>
       </c>
@@ -4321,6 +4632,16 @@
       <c r="F32">
         <v>0</v>
       </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N32" t="s">
         <v>184</v>
       </c>
@@ -4401,6 +4722,16 @@
       <c r="F33">
         <v>1</v>
       </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O33">
         <v>1</v>
       </c>
@@ -4466,6 +4797,16 @@
       <c r="F34">
         <v>1</v>
       </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O34">
         <v>1</v>
       </c>
@@ -4531,6 +4872,16 @@
       <c r="F35">
         <v>1</v>
       </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O35">
         <v>1</v>
       </c>
@@ -4596,6 +4947,16 @@
       <c r="F36">
         <v>1</v>
       </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O36">
         <v>1</v>
       </c>
@@ -4661,6 +5022,16 @@
       <c r="F37">
         <v>0</v>
       </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N37" t="s">
         <v>192</v>
       </c>
@@ -4741,6 +5112,16 @@
       <c r="F38">
         <v>1</v>
       </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O38">
         <v>1</v>
       </c>
@@ -4818,6 +5199,16 @@
       <c r="F39">
         <v>1</v>
       </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O39">
         <v>1</v>
       </c>
@@ -4883,6 +5274,16 @@
       <c r="F40">
         <v>1</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N40" t="s">
         <v>152</v>
       </c>
@@ -4951,6 +5352,16 @@
       <c r="F41">
         <v>1</v>
       </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O41">
         <v>1</v>
       </c>
@@ -5028,6 +5439,16 @@
       <c r="F42">
         <v>1</v>
       </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O42">
         <v>1</v>
       </c>
@@ -5105,6 +5526,16 @@
       <c r="F43">
         <v>0</v>
       </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N43" t="s">
         <v>206</v>
       </c>
@@ -5185,6 +5616,16 @@
       <c r="F44">
         <v>1</v>
       </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O44">
         <v>1</v>
       </c>
@@ -5223,6 +5664,16 @@
       <c r="F45">
         <v>1</v>
       </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O45">
         <v>1</v>
       </c>
@@ -5261,6 +5712,16 @@
       <c r="F46">
         <v>0</v>
       </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N46" t="s">
         <v>218</v>
       </c>
@@ -5302,6 +5763,16 @@
       <c r="F47">
         <v>1</v>
       </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N47" t="s">
         <v>221</v>
       </c>
@@ -5343,6 +5814,16 @@
       <c r="F48">
         <v>1</v>
       </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N48" t="s">
         <v>221</v>
       </c>
@@ -5384,6 +5865,16 @@
       <c r="F49">
         <v>0</v>
       </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N49" t="s">
         <v>36</v>
       </c>
@@ -5425,6 +5916,16 @@
       <c r="F50">
         <v>0</v>
       </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N50" t="s">
         <v>36</v>
       </c>
@@ -5466,6 +5967,16 @@
       <c r="F51">
         <v>1</v>
       </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O51">
         <v>1</v>
       </c>
@@ -5504,6 +6015,16 @@
       <c r="F52">
         <v>1</v>
       </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="O52">
         <v>1</v>
       </c>
@@ -5542,6 +6063,16 @@
       <c r="F53">
         <v>1</v>
       </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N53" t="s">
         <v>231</v>
       </c>
@@ -5622,6 +6153,16 @@
       <c r="F54">
         <v>1</v>
       </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N54" t="s">
         <v>231</v>
       </c>
@@ -5702,6 +6243,16 @@
       <c r="F55">
         <v>1</v>
       </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N55" t="s">
         <v>231</v>
       </c>
@@ -5782,6 +6333,16 @@
       <c r="F56">
         <v>1</v>
       </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N56" t="s">
         <v>231</v>
       </c>
@@ -5850,6 +6411,16 @@
       <c r="F57">
         <v>1</v>
       </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N57" t="s">
         <v>231</v>
       </c>
@@ -5930,6 +6501,16 @@
       <c r="F58">
         <v>1</v>
       </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <f>F58</f>
+        <v>1</v>
+      </c>
       <c r="N58" t="s">
         <v>231</v>
       </c>
@@ -7586,7 +8167,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>310</v>
       </c>

</xml_diff>